<commit_message>
Added exception screenshots on init
</commit_message>
<xml_diff>
--- a/Config Template.xlsx
+++ b/Config Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heiner.monge\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heiner.monge\Documents\UiPath\ModifiedREFramework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0811A74B-0A6B-4FC6-A2C7-3F5170411AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3D2769-8CE1-4234-907F-5A0CF6CAEAE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -40,15 +40,6 @@
   </si>
   <si>
     <t>MaxRetryNumber</t>
-  </si>
-  <si>
-    <t>ExScreenshotsFolderPath</t>
-  </si>
-  <si>
-    <t>Exceptions_Screenshots</t>
-  </si>
-  <si>
-    <t>Where to save exceptions screenshots - can be a full or a relative path.</t>
   </si>
   <si>
     <t>LogMessage_GetTransactionData</t>
@@ -637,34 +628,34 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1681,10 +1672,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z24"/>
+  <dimension ref="A1:Z22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -1737,18 +1728,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -1759,149 +1750,138 @@
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
+      <c r="A6" t="s">
         <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:26">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="30">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="30">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="30">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="30">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="30">
       <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>42</v>
+        <v>31</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="30">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="45">
+      <c r="A15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" ht="30">
-      <c r="A14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="30">
-      <c r="A15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15">
-        <v>3</v>
+      <c r="B15" t="b">
+        <v>1</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" t="b">
-        <v>1</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="45">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>59</v>
-      </c>
-      <c r="B20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="45">
-      <c r="A22" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24">
-        <v>3</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1934,7 +1914,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -1964,24 +1944,24 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>